<commit_message>
fix: Register ISponsorDealerAnalyticsCacheService in PlantAnalysisWorkerService
- Added missing Analytics Cache Service DI registration
- Fixes bulk dealer invitation processing error
- CreateDealerInvitationCommandHandler now properly resolves dependencies
- Error: 'Unable to resolve service ISponsorDealerAnalyticsCacheService' resolved
</commit_message>
<xml_diff>
--- a/claudedocs/Dealers/1_basic_example.xlsx
+++ b/claudedocs/Dealers/1_basic_example.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Email</t>
   </si>
@@ -33,86 +33,20 @@
     <t>CodeCount</t>
   </si>
   <si>
-    <t>ahmet.yilmaz@example.com</t>
+    <t>ziraai@ziraat.com</t>
   </si>
   <si>
-    <t>mehmet.kaya@example.com</t>
+    <t>905421396386</t>
   </si>
   <si>
-    <t>Mehmet Kaya</t>
-  </si>
-  <si>
-    <t>ayse.demir@example.com</t>
-  </si>
-  <si>
-    <t>fatma.ozturk@example.com</t>
-  </si>
-  <si>
-    <t>ali.celik@example.com</t>
-  </si>
-  <si>
-    <t>zeynep.sahin@example.com</t>
-  </si>
-  <si>
-    <t>mustafa.yildiz@example.com</t>
-  </si>
-  <si>
-    <t>elif.arslan@example.com</t>
-  </si>
-  <si>
-    <t>Elif Arslan</t>
-  </si>
-  <si>
-    <t>hasan.koc@example.com</t>
-  </si>
-  <si>
-    <t>selin.aydin@example.com</t>
-  </si>
-  <si>
-    <t>Ahmet Yılmaz</t>
-  </si>
-  <si>
-    <t>905551234567</t>
-  </si>
-  <si>
-    <t>905554567890</t>
-  </si>
-  <si>
-    <t>905555678901</t>
-  </si>
-  <si>
-    <t>905558901234</t>
-  </si>
-  <si>
-    <t>905559012345</t>
-  </si>
-  <si>
-    <t>Ayşe Aydemiz</t>
-  </si>
-  <si>
-    <t>Fatma Zehra</t>
-  </si>
-  <si>
-    <t>Ali Çelik</t>
-  </si>
-  <si>
-    <t>Zeynep Şahin</t>
-  </si>
-  <si>
-    <t>Mustafa Ali</t>
-  </si>
-  <si>
-    <t>Hasan Koş</t>
-  </si>
-  <si>
-    <t>Selin Aydın</t>
+    <t>Tolga KAYA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +177,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -545,7 +487,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -588,12 +530,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="%20 - Vurgu1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="%20 - Vurgu2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="%20 - Vurgu3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -624,6 +568,7 @@
     <cellStyle name="Hesaplama" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="İşaretli Hücre" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="İyi" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Köprü" xfId="42" builtinId="8"/>
     <cellStyle name="Kötü" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Not" xfId="15" builtinId="10" customBuiltin="1"/>
@@ -916,7 +861,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,147 +886,51 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>5552345678</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <v>5553456789</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1">
-        <v>5556789012</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1">
-        <v>5557890123</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="1">
-        <v>5550123456</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11">
-        <v>7</v>
-      </c>
+      <c r="B11" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: Register IDealerInvitationConfigurationService in PlantAnalysisWorkerService
Resolves MediatR handler activation error when processing bulk dealer invitations with SMS.

🐛 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/claudedocs/Dealers/1_basic_example.xlsx
+++ b/claudedocs/Dealers/1_basic_example.xlsx
@@ -33,13 +33,13 @@
     <t>CodeCount</t>
   </si>
   <si>
-    <t>ziraai@ziraat.com</t>
-  </si>
-  <si>
     <t>905421396386</t>
   </si>
   <si>
     <t>Tolga KAYA</t>
+  </si>
+  <si>
+    <t>ziraai@ziraai.com</t>
   </si>
 </sst>
 </file>
@@ -861,7 +861,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,13 +887,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
       <c r="D2">
         <v>12</v>

</xml_diff>